<commit_message>
Add color spectrum filtering
</commit_message>
<xml_diff>
--- a/Docs/snake-curves-from-paper-csv.xlsx
+++ b/Docs/snake-curves-from-paper-csv.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\RgbToSpectrum\Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10848"/>
+    <workbookView xWindow="2130" yWindow="2175" windowWidth="23040" windowHeight="10845"/>
   </bookViews>
   <sheets>
     <sheet name="snake-curves-from-paper" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Values R</t>
   </si>
@@ -42,16 +37,28 @@
     <t>values W</t>
     <phoneticPr fontId="18"/>
   </si>
+  <si>
+    <t>Lambdas</t>
+  </si>
+  <si>
+    <t>Spectra</t>
+  </si>
+  <si>
+    <t>Transmittances</t>
+  </si>
+  <si>
+    <t>Warming filter 85</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -59,7 +66,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -67,7 +74,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="major"/>
@@ -76,7 +83,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -85,7 +92,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -94,7 +101,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -102,7 +109,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -110,7 +117,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -118,7 +125,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -126,7 +133,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -135,7 +142,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -144,7 +151,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -152,7 +159,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -161,7 +168,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -169,7 +176,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -178,7 +185,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -187,7 +194,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -195,17 +202,24 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="33">
@@ -633,8 +647,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -950,7 +968,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -958,488 +976,765 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:AF14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>361.85599999999999</v>
+      </c>
+      <c r="C2">
+        <v>383.505</v>
+      </c>
+      <c r="D2">
+        <v>405.15499999999997</v>
+      </c>
+      <c r="E2">
+        <v>426.80399999999997</v>
+      </c>
+      <c r="F2">
+        <v>448.45400000000001</v>
+      </c>
+      <c r="G2">
+        <v>470.10300000000001</v>
+      </c>
+      <c r="H2">
+        <v>491.75299999999999</v>
+      </c>
+      <c r="I2">
+        <v>513.40200000000004</v>
+      </c>
+      <c r="J2">
+        <v>535.05200000000002</v>
+      </c>
+      <c r="K2">
+        <v>556.70100000000002</v>
+      </c>
+      <c r="L2">
+        <v>578.351</v>
+      </c>
+      <c r="M2">
+        <v>600</v>
+      </c>
+      <c r="N2">
+        <v>621.649</v>
+      </c>
+      <c r="O2">
+        <v>643.29899999999998</v>
+      </c>
+      <c r="P2">
+        <v>664.94799999999998</v>
+      </c>
+      <c r="Q2">
+        <v>686.59799999999996</v>
+      </c>
+      <c r="R2">
+        <v>708.24699999999996</v>
+      </c>
+      <c r="S2">
+        <v>729.89700000000005</v>
+      </c>
+      <c r="T2">
+        <v>751.54600000000005</v>
+      </c>
+      <c r="U2">
+        <v>773.19600000000003</v>
+      </c>
+      <c r="V2">
+        <v>794.84500000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
         <v>9.5589999999999994E-2</v>
       </c>
-      <c r="C1">
+      <c r="C3">
         <v>9.5589999999999994E-2</v>
       </c>
-      <c r="D1">
+      <c r="D3">
         <v>8.8239999999999999E-2</v>
       </c>
-      <c r="E1">
+      <c r="E3">
         <v>7.3529999999999998E-2</v>
       </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>0</v>
-      </c>
-      <c r="J1">
-        <v>0</v>
-      </c>
-      <c r="K1">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>8.8239999999999999E-2</v>
       </c>
-      <c r="L1">
+      <c r="L3">
         <v>0.69852999999999998</v>
       </c>
-      <c r="M1">
-        <v>1</v>
-      </c>
-      <c r="N1">
-        <v>1</v>
-      </c>
-      <c r="O1">
-        <v>1</v>
-      </c>
-      <c r="P1">
-        <v>1</v>
-      </c>
-      <c r="Q1">
-        <v>1</v>
-      </c>
-      <c r="R1">
-        <v>1</v>
-      </c>
-      <c r="S1">
-        <v>1</v>
-      </c>
-      <c r="T1">
-        <v>1</v>
-      </c>
-      <c r="U1">
-        <v>1</v>
-      </c>
-      <c r="V1">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
+    <row r="4" spans="1:32">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>3.6760000000000001E-2</v>
       </c>
-      <c r="G2">
+      <c r="G4">
         <v>0.38971</v>
       </c>
-      <c r="H2">
+      <c r="H4">
         <v>0.78676000000000001</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
         <v>0.77941000000000005</v>
       </c>
-      <c r="L2">
+      <c r="L4">
         <v>0.31618000000000002</v>
       </c>
-      <c r="M2">
+      <c r="M4">
         <v>7.3499999999999998E-3</v>
       </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="5" spans="1:32">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B5">
         <v>0.99265000000000003</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>0.86765000000000003</v>
       </c>
-      <c r="G3">
+      <c r="G5">
         <v>0.61029</v>
       </c>
-      <c r="H3">
+      <c r="H5">
         <v>0.30881999999999998</v>
       </c>
-      <c r="I3">
+      <c r="I5">
         <v>8.0879999999999994E-2</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
         <v>2.9409999999999999E-2</v>
       </c>
-      <c r="N3">
+      <c r="N5">
         <v>5.1470000000000002E-2</v>
       </c>
-      <c r="O3">
+      <c r="O5">
         <v>6.6180000000000003E-2</v>
       </c>
-      <c r="P3">
+      <c r="P5">
         <v>6.6180000000000003E-2</v>
       </c>
-      <c r="Q3">
+      <c r="Q5">
         <v>6.6180000000000003E-2</v>
       </c>
-      <c r="R3">
+      <c r="R5">
         <v>6.6180000000000003E-2</v>
       </c>
-      <c r="S3">
+      <c r="S5">
         <v>6.6180000000000003E-2</v>
       </c>
-      <c r="T3">
+      <c r="T5">
         <v>6.6180000000000003E-2</v>
       </c>
-      <c r="U3">
+      <c r="U5">
         <v>6.6180000000000003E-2</v>
       </c>
-      <c r="V3">
+      <c r="V5">
         <v>6.6180000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="6" spans="1:32">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>0.99265000000000003</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>0.99265000000000003</v>
       </c>
-      <c r="D4">
+      <c r="D6">
         <v>0.98529</v>
       </c>
-      <c r="E4">
+      <c r="E6">
         <v>0.92647000000000002</v>
       </c>
-      <c r="F4">
+      <c r="F6">
         <v>0.98529</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
         <v>0.91912000000000005</v>
       </c>
-      <c r="L4">
+      <c r="L6">
         <v>0.30147000000000002</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
         <v>7.3499999999999998E-3</v>
       </c>
-      <c r="S4">
+      <c r="S6">
         <v>7.3499999999999998E-3</v>
       </c>
-      <c r="T4">
+      <c r="T6">
         <v>7.3499999999999998E-3</v>
       </c>
-      <c r="U4">
+      <c r="U6">
         <v>7.3499999999999998E-3</v>
       </c>
-      <c r="V4">
+      <c r="V6">
         <v>7.3499999999999998E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="7" spans="1:32">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
         <v>0.97794000000000003</v>
       </c>
-      <c r="G5">
+      <c r="G7">
         <v>0.61765000000000003</v>
       </c>
-      <c r="H5">
+      <c r="H7">
         <v>0.19853000000000001</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
         <v>0.24265</v>
       </c>
-      <c r="L5">
+      <c r="L7">
         <v>0.68381999999999998</v>
       </c>
-      <c r="M5">
+      <c r="M7">
         <v>0.98529</v>
       </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5">
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
         <v>0.99265000000000003</v>
       </c>
-      <c r="R5">
+      <c r="R7">
         <v>0.97794000000000003</v>
       </c>
-      <c r="S5">
+      <c r="S7">
         <v>0.97794000000000003</v>
       </c>
-      <c r="T5">
+      <c r="T7">
         <v>0.98529</v>
       </c>
-      <c r="U5">
+      <c r="U7">
         <v>0.98529</v>
       </c>
-      <c r="V5">
+      <c r="V7">
         <v>0.98529</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="8" spans="1:32">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>7.3499999999999998E-3</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>7.3499999999999998E-3</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>0.30147000000000002</v>
       </c>
-      <c r="G6">
+      <c r="G8">
         <v>0.39706000000000002</v>
       </c>
-      <c r="H6">
+      <c r="H8">
         <v>0.69852999999999998</v>
       </c>
-      <c r="I6">
+      <c r="I8">
         <v>0.92647000000000002</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
         <v>0.97058999999999995</v>
       </c>
-      <c r="N6">
+      <c r="N8">
         <v>0.95587999999999995</v>
       </c>
-      <c r="O6">
+      <c r="O8">
         <v>0.95587999999999995</v>
       </c>
-      <c r="P6">
+      <c r="P8">
         <v>0.95587999999999995</v>
       </c>
-      <c r="Q6">
+      <c r="Q8">
         <v>0.96323999999999999</v>
       </c>
-      <c r="R6">
+      <c r="R8">
         <v>0.97058999999999995</v>
       </c>
-      <c r="S6">
+      <c r="S8">
         <v>0.98529</v>
       </c>
-      <c r="T6">
+      <c r="T8">
         <v>0.99265000000000003</v>
       </c>
-      <c r="U6">
-        <v>1</v>
-      </c>
-      <c r="V6">
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="9" spans="1:32">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B9">
         <v>0.98750000000000004</v>
       </c>
-      <c r="C7">
+      <c r="C9">
         <v>0.99553999999999998</v>
       </c>
-      <c r="D7">
+      <c r="D9">
         <v>1.05714</v>
       </c>
-      <c r="E7">
+      <c r="E9">
         <v>1.07589</v>
       </c>
-      <c r="F7">
+      <c r="F9">
         <v>0.89642999999999995</v>
       </c>
-      <c r="G7">
+      <c r="G9">
         <v>0.99553999999999998</v>
       </c>
-      <c r="H7">
+      <c r="H9">
         <v>1.1160699999999999</v>
       </c>
-      <c r="I7">
+      <c r="I9">
         <v>1.07857</v>
       </c>
-      <c r="J7">
+      <c r="J9">
         <v>1.0008900000000001</v>
       </c>
-      <c r="K7">
+      <c r="K9">
         <v>0.84286000000000005</v>
       </c>
-      <c r="L7">
+      <c r="L9">
         <v>1.0196400000000001</v>
       </c>
-      <c r="M7">
+      <c r="M9">
         <v>1.04643</v>
       </c>
-      <c r="N7">
+      <c r="N9">
         <v>1.05179</v>
       </c>
-      <c r="O7">
+      <c r="O9">
         <v>1.0625</v>
       </c>
-      <c r="P7">
+      <c r="P9">
         <v>1.06518</v>
       </c>
-      <c r="Q7">
+      <c r="Q9">
         <v>1.06518</v>
       </c>
-      <c r="R7">
+      <c r="R9">
         <v>1.0625</v>
       </c>
-      <c r="S7">
+      <c r="S9">
         <v>1.06518</v>
       </c>
-      <c r="T7">
+      <c r="T9">
         <v>1.06786</v>
       </c>
-      <c r="U7">
+      <c r="U9">
         <v>1.06786</v>
       </c>
-      <c r="V7">
+      <c r="V9">
         <v>1.06518</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1">
+        <v>400</v>
+      </c>
+      <c r="C13" s="1">
+        <v>410</v>
+      </c>
+      <c r="D13" s="1">
+        <v>420</v>
+      </c>
+      <c r="E13" s="1">
+        <v>430</v>
+      </c>
+      <c r="F13" s="1">
+        <v>440</v>
+      </c>
+      <c r="G13" s="1">
+        <v>450</v>
+      </c>
+      <c r="H13" s="1">
+        <v>460</v>
+      </c>
+      <c r="I13" s="1">
+        <v>470</v>
+      </c>
+      <c r="J13" s="1">
+        <v>480</v>
+      </c>
+      <c r="K13" s="1">
+        <v>490</v>
+      </c>
+      <c r="L13" s="1">
+        <v>500</v>
+      </c>
+      <c r="M13" s="1">
+        <v>510</v>
+      </c>
+      <c r="N13" s="1">
+        <v>520</v>
+      </c>
+      <c r="O13" s="1">
+        <v>530</v>
+      </c>
+      <c r="P13" s="1">
+        <v>540</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>550</v>
+      </c>
+      <c r="R13" s="1">
+        <v>560</v>
+      </c>
+      <c r="S13" s="1">
+        <v>570</v>
+      </c>
+      <c r="T13" s="1">
+        <v>580</v>
+      </c>
+      <c r="U13" s="1">
+        <v>590</v>
+      </c>
+      <c r="V13" s="1">
+        <v>600</v>
+      </c>
+      <c r="W13" s="1">
+        <v>610</v>
+      </c>
+      <c r="X13" s="1">
+        <v>620</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>630</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>640</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>650</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>660</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>670</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>680</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>690</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="R14" s="2">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="T14" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="U14" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="V14" s="2">
+        <v>0.872</v>
+      </c>
+      <c r="W14" s="2">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="X14" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="AD14" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="AE14" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="AF14" s="2">
+        <v>0.91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>